<commit_message>
Implement website scanning process
</commit_message>
<xml_diff>
--- a/files/scan_websites_list_template.xlsx
+++ b/files/scan_websites_list_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\_data\dataguard\target-list-tool\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EDCAA3-DB4A-4AD9-8E15-6CBA3F4343BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA07CC8-D179-4003-AB55-4E907D9DA936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{653AAF79-0B76-44CE-86C5-4E92D0C34510}"/>
   </bookViews>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Company</t>
+    <t>Website</t>
   </si>
   <si>
-    <t>Website</t>
+    <t>Account</t>
   </si>
 </sst>
 </file>
@@ -420,9 +420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E31A063-3783-4B9E-97F0-024CE52AA00F}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -431,10 +429,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>